<commit_message>
Two lightning elementals added
</commit_message>
<xml_diff>
--- a/GameMasterGuide/Data/Beasts/Species.xlsx
+++ b/GameMasterGuide/Data/Beasts/Species.xlsx
@@ -11,9 +11,9 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$54</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Extract" vbProcedure="false">Sheet1!$A$2:$A$166</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -288,6 +288,13 @@
   </si>
   <si>
     <t xml:space="preserve">Wyverns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electric Elemental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Within the \imp{Elemental Planes} there can be found a single, enormous mountain, surrounded at all times by a roiling, black cloud filled with crackling energy: \key{Thundertop}. Lightning and thunder are everpresent in this hostile environment, and every surface is highly charged with static electricity – the foolish explorer who sets foot on the mountain of thunder without some rubber-soled boots is liable to have a {\it very} bad time. 
+Within the crackling chaos and the booming crashes of this formiddable environment, reside a number of creatures who have learned to harness, channel and consume electrical energy, using it for their own end - \key{Electric Elementals}. </t>
   </si>
 </sst>
 </file>
@@ -421,10 +428,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -843,8 +850,16 @@
         <v>71</v>
       </c>
     </row>
+    <row r="55" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B1"/>
+  <autoFilter ref="A1:B54"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Cosmology continues + creations added
</commit_message>
<xml_diff>
--- a/GameMasterGuide/Data/Beasts/Species.xlsx
+++ b/GameMasterGuide/Data/Beasts/Species.xlsx
@@ -11,9 +11,9 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$54</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Extract" vbProcedure="false">Sheet1!$A$2:$A$166</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -116,25 +116,29 @@
     <t xml:space="preserve">Creations</t>
   </si>
   <si>
+    <t xml:space="preserve">\key{Creations} are a class of magical creature which have, either through accident or design, been created by artificial means. This is usually the result of (highly illegal) experimental breeding, though direct magical manipulation of a species has been known to occur. 
+Almost every beginner \imp{Transfiguration} student has, at some point, been responsible for the creation of a pseudo-\imp{Creation}, when they accidentaly morphed their pet rat into a rat-goblet, or some other ungodly accident. What sets the creatures below apart from these short-lived accidents is that \imp{Creations} are a viable species in their own right, with the ability to reproduce and continue their species’ existence, and they have often escaped from their creators’ control, and have made their home somewhere in the magical world. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demiguise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dinosaurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long thought extinct by the muggles, dinosaurs are a class of ancient lizard and reptilian creatures which dominated life on Earth up until 75 million years ago. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dragons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elemental Avatar</t>
+  </si>
+  <si>
     <t xml:space="preserve">b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demiguise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dinosaurs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Long thought extinct by the muggles, dinosaurs are a class of ancient lizard and reptilian creatures which dominated life on Earth up until 75 million years ago. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dragons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elemental Avatar</t>
   </si>
   <si>
     <t xml:space="preserve">Elf</t>
@@ -436,8 +440,8 @@
   </sheetPr>
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -528,7 +532,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
@@ -565,36 +569,36 @@
         <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="281.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>26</v>
@@ -602,31 +606,31 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="359.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>26</v>
@@ -634,23 +638,23 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>26</v>
@@ -658,23 +662,23 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>26</v>
@@ -682,31 +686,31 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>26</v>
@@ -714,23 +718,23 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>26</v>
@@ -738,15 +742,15 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>26</v>
@@ -754,15 +758,15 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>26</v>
@@ -770,31 +774,31 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>26</v>
@@ -802,78 +806,78 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="270.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1"/>
+  <autoFilter ref="A1:B54"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Elves added + hogwarts expanded
</commit_message>
<xml_diff>
--- a/GameMasterGuide/Data/Beasts/Species.xlsx
+++ b/GameMasterGuide/Data/Beasts/Species.xlsx
@@ -11,9 +11,9 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$54</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Extract" vbProcedure="false">Sheet1!$A$2:$A$166</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$54</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -141,7 +141,7 @@
     <t xml:space="preserve">b</t>
   </si>
   <si>
-    <t xml:space="preserve">Elf</t>
+    <t xml:space="preserve">Elves</t>
   </si>
   <si>
     <t xml:space="preserve">Modern muggle culture frequently imagines Elves to be superhuman, immortal and otherworldly creatures – outwardly appearing as impossibly beautiful humans and wielding immense, primal magic. This is primarly due to the influence of the muggle writer Tolkein (who was himself a squib). In reality, elves are much closer to those envisaged in medieval Germanic mythology – small, impish tricksters. 
@@ -441,7 +441,7 @@
   <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -877,7 +877,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B54"/>
+  <autoFilter ref="A1:B1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>